<commit_message>
modified figures 3 and S2
</commit_message>
<xml_diff>
--- a/output/glm_results.xlsx
+++ b/output/glm_results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="540" windowWidth="24780" windowHeight="8040" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="0" windowWidth="14040" windowHeight="7180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="glm_results.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Modnames</t>
   </si>
@@ -96,12 +96,27 @@
   <si>
     <t>Cumulative weight</t>
   </si>
+  <si>
+    <r>
+      <t>AIC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +155,22 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,8 +198,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -195,7 +240,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,14 +586,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="6" customWidth="1"/>
     <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -576,9 +635,8 @@
         <f t="shared" ref="L1:M2" si="0">C1</f>
         <v>K</v>
       </c>
-      <c r="M1" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>AIC</v>
+      <c r="M1" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>14</v>
@@ -683,7 +741,7 @@
         <v>-35.189529538224399</v>
       </c>
       <c r="I3">
-        <v>0.92830213547163098</v>
+        <v>0.92830213547162999</v>
       </c>
       <c r="K3" s="6" t="str">
         <f t="shared" si="1"/>
@@ -854,13 +912,13 @@
         <v>80.233702394867606</v>
       </c>
       <c r="E6">
-        <v>7.73460961736677</v>
+        <v>7.7346096173667602</v>
       </c>
       <c r="F6">
-        <v>2.09146625476593E-2</v>
+        <v>2.0914662547659502E-2</v>
       </c>
       <c r="G6">
-        <v>1.39613443034099E-2</v>
+        <v>1.3961344303410001E-2</v>
       </c>
       <c r="H6">
         <v>-33.116851197433803</v>
@@ -903,6 +961,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>